<commit_message>
SE ACTUALIZA FORMATO DE SEGUIMIENTO SPRINT 4 CON LA DISTRIBUCION DE ACTIVIDADES
</commit_message>
<xml_diff>
--- a/SPRINT4/FORMATO SEGUIMIENTO-SPRINT4.xlsx
+++ b/SPRINT4/FORMATO SEGUIMIENTO-SPRINT4.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Desarrollo Modulo Equipo (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>HELVER ROA</t>
   </si>
 </sst>
 </file>
@@ -737,6 +740,106 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,106 +867,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,6 +884,57 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -952,57 +1006,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1066,15 +1069,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Distribucion" displayName="Distribucion" ref="A1:F9" totalsRowCount="1" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Distribucion" displayName="Distribucion" ref="A1:F9" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="16"/>
-    <tableColumn id="5" name="VALOR" dataDxfId="15" totalsRowDxfId="3" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="14" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="RESPONSABLE" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="3" name="ESTADO" dataDxfId="12"/>
-    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="1" name="ID" dataDxfId="9"/>
+    <tableColumn id="5" name="VALOR" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="RESPONSABLE" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="5"/>
+    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1378,230 +1381,230 @@
       <c r="E1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="29">
         <v>44816</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="50"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="57"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
       <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="51"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="58"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
       <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="51"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="58"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="51"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="58"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="51"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="58"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="52"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="53"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="51"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="58"/>
       <c r="G9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="51"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="58"/>
       <c r="G10" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="66">
         <v>44819</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="51"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="58"/>
       <c r="G11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="51"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="52"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="46"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="42"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="47"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="42"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="47"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="42"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="47"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="42"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="47"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="43"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="46"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="42"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="47"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="42"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="47"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="42"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="47"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="42"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="47"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="43"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="48"/>
       <c r="G25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1609,66 +1612,70 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="67"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="46"/>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="42"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="47"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="42"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="47"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="42"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="47"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="68"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="42"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="47"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="69"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="43"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
     <mergeCell ref="E20:E25"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -1685,27 +1692,23 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B8:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1717,7 +1720,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1779,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="5" t="str">
@@ -1827,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="str">
@@ -1857,7 +1860,7 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="70"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="27" t="s">
         <v>42</v>
       </c>
@@ -1975,28 +1978,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E7 E2">
-    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SE ANEXA CREACION FRONT-END ENTIDAD PROVEEDORES
</commit_message>
<xml_diff>
--- a/SPRINT4/FORMATO SEGUIMIENTO-SPRINT4.xlsx
+++ b/SPRINT4/FORMATO SEGUIMIENTO-SPRINT4.xlsx
@@ -13,10 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="INFORME SPRINT" sheetId="12" r:id="rId1"/>
-    <sheet name="SEGUIMIENTO 21-09-2022" sheetId="19" r:id="rId2"/>
-    <sheet name="SEGUIMIENTO 20-09-2022" sheetId="18" r:id="rId3"/>
-    <sheet name="TUTORIA 15-09-2022" sheetId="17" r:id="rId4"/>
-    <sheet name="DISTRIBUCION 05-09-2022" sheetId="16" r:id="rId5"/>
+    <sheet name="SEGUIMIENTO 26-09-2022" sheetId="21" r:id="rId2"/>
+    <sheet name="SEGUIMIENTO 25-09-2022" sheetId="20" r:id="rId3"/>
+    <sheet name="SEGUIMIENTO 21-09-2022" sheetId="19" r:id="rId4"/>
+    <sheet name="SEGUIMIENTO 20-09-2022" sheetId="18" r:id="rId5"/>
+    <sheet name="TUTORIA 15-09-2022" sheetId="17" r:id="rId6"/>
+    <sheet name="DISTRIBUCION 05-09-2022" sheetId="16" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -175,6 +177,12 @@
   </si>
   <si>
     <t>SEGUIMIENTO 2</t>
+  </si>
+  <si>
+    <t>SEGUIMIENTO 3</t>
+  </si>
+  <si>
+    <t>SEGUIMIENTO 4</t>
   </si>
 </sst>
 </file>
@@ -890,7 +898,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="112">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1028,19 +1036,13 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1051,6 +1053,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1058,6 +1063,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1089,46 +1097,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1262,6 +1230,46 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1395,6 +1403,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -1432,6 +1470,202 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1676,11 +1910,87 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>39655</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2702718</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>354242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9469405" y="9929813"/>
+          <a:ext cx="2663063" cy="1497242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>39376</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2702719</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>44837</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9469126" y="12287251"/>
+          <a:ext cx="2663343" cy="1497399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Distribucion245" displayName="Distribucion245" ref="A1:F9" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Distribucion24567" displayName="Distribucion24567" ref="A1:F9" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="9"/>
@@ -1689,6 +1999,40 @@
     <tableColumn id="6" name="RESPONSABLE" dataDxfId="3" totalsRowDxfId="4"/>
     <tableColumn id="3" name="ESTADO" dataDxfId="2"/>
     <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Distribucion2456" displayName="Distribucion2456" ref="A1:F9" totalsRowCount="1" headerRowDxfId="104">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="103"/>
+    <tableColumn id="5" name="VALOR" dataDxfId="102" totalsRowDxfId="101" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="100" totalsRowDxfId="99"/>
+    <tableColumn id="6" name="RESPONSABLE" dataDxfId="98" totalsRowDxfId="97"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="96"/>
+    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="95" totalsRowDxfId="94" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Distribucion245" displayName="Distribucion245" ref="A1:F9" totalsRowCount="1" headerRowDxfId="86">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="85"/>
+    <tableColumn id="5" name="VALOR" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="82" totalsRowDxfId="81"/>
+    <tableColumn id="6" name="RESPONSABLE" dataDxfId="80" totalsRowDxfId="79"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="78"/>
+    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="76" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1696,25 +2040,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Distribucion24" displayName="Distribucion24" ref="A1:F9" totalsRowCount="1" headerRowDxfId="28">
-  <autoFilter ref="A1:F8"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="27"/>
-    <tableColumn id="5" name="VALOR" dataDxfId="26" totalsRowDxfId="21" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="25" totalsRowDxfId="20"/>
-    <tableColumn id="6" name="RESPONSABLE" dataDxfId="24" totalsRowDxfId="19"/>
-    <tableColumn id="3" name="ESTADO" dataDxfId="23"/>
-    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="18" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Distribucion2" displayName="Distribucion2" ref="A1:F9" totalsRowCount="1" headerRowDxfId="68">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Distribucion24" displayName="Distribucion24" ref="A1:F9" totalsRowCount="1" headerRowDxfId="68">
   <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="67"/>
@@ -1723,6 +2050,23 @@
     <tableColumn id="6" name="RESPONSABLE" dataDxfId="62" totalsRowDxfId="61"/>
     <tableColumn id="3" name="ESTADO" dataDxfId="60"/>
     <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Distribucion2" displayName="Distribucion2" ref="A1:F9" totalsRowCount="1" headerRowDxfId="46">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="45"/>
+    <tableColumn id="5" name="VALOR" dataDxfId="44" totalsRowDxfId="43" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="6" name="RESPONSABLE" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="38"/>
+    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1730,16 +2074,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Distribucion" displayName="Distribucion" ref="A1:F9" totalsRowCount="1" headerRowDxfId="50">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Distribucion" displayName="Distribucion" ref="A1:F9" totalsRowCount="1" headerRowDxfId="28">
   <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="49"/>
-    <tableColumn id="5" name="VALOR" dataDxfId="48" totalsRowDxfId="47" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="6" name="RESPONSABLE" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="3" name="ESTADO" dataDxfId="42"/>
-    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40" dataCellStyle="Porcentaje">
+    <tableColumn id="1" name="ID" dataDxfId="27"/>
+    <tableColumn id="5" name="VALOR" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="6" name="RESPONSABLE" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="20"/>
+    <tableColumn id="4" name="PROGRESO" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2010,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,8 +2630,12 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="29">
+        <v>44829</v>
+      </c>
       <c r="C26" s="44"/>
       <c r="D26" s="44"/>
       <c r="E26" s="46"/>
@@ -2327,8 +2675,63 @@
       <c r="D31" s="50"/>
       <c r="E31" s="48"/>
     </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="29">
+        <v>44830</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="46"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="47"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="47"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="47"/>
+    </row>
+    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="34"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="63">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
@@ -2393,7 +2796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2442,7 +2845,7 @@
         <v>47</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2461,7 +2864,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2480,7 +2883,7 @@
         <v>47</v>
       </c>
       <c r="F4" s="5" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2499,7 +2902,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2518,7 +2921,7 @@
         <v>47</v>
       </c>
       <c r="F6" s="5" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="6"/>
@@ -2538,7 +2941,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="26" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2557,7 +2960,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="26" t="str">
-        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion24567[[#This Row],[ESTADO]]="HECHO",Distribucion24567[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2566,7 +2969,7 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="F9" s="6">
-        <f>SUBTOTAL(109,Distribucion245[PROGRESO])</f>
+        <f>SUBTOTAL(109,Distribucion24567[PROGRESO])</f>
         <v>0</v>
       </c>
     </row>
@@ -2575,7 +2978,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="2">
-        <f>COUNTIF(Distribucion245[ESTADO],"HACER")</f>
+        <f>COUNTIF(Distribucion24567[ESTADO],"HACER")</f>
         <v>0</v>
       </c>
       <c r="G11" s="16" t="s">
@@ -2593,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="2">
-        <f>COUNTIF(Distribucion245[ESTADO],"HACIENDO")</f>
+        <f>COUNTIF(Distribucion24567[ESTADO],"HACIENDO")</f>
         <v>7</v>
       </c>
       <c r="G12" s="20">
@@ -2611,7 +3014,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <f>COUNTIF(Distribucion245[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Distribucion24567[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="G13" s="20">
@@ -2629,7 +3032,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2">
-        <f>COUNTIF(Distribucion245[ESTADO],"HECHO")</f>
+        <f>COUNTIF(Distribucion24567[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
       <c r="G14" s="20">
@@ -2647,7 +3050,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="2">
-        <f>COUNTIF(Distribucion245[ESTADO],"POSPUESTO")</f>
+        <f>COUNTIF(Distribucion24567[ESTADO],"POSPUESTO")</f>
         <v>0</v>
       </c>
       <c r="G15" s="20">
@@ -2760,7 +3163,7 @@
         <v>47</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2779,7 +3182,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2798,7 +3201,7 @@
         <v>47</v>
       </c>
       <c r="F4" s="5" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2817,7 +3220,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2836,7 +3239,7 @@
         <v>47</v>
       </c>
       <c r="F6" s="5" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="6"/>
@@ -2856,7 +3259,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="26" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2875,7 +3278,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="26" t="str">
-        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion2456[[#This Row],[ESTADO]]="HECHO",Distribucion2456[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2884,7 +3287,7 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="F9" s="6">
-        <f>SUBTOTAL(109,Distribucion24[PROGRESO])</f>
+        <f>SUBTOTAL(109,Distribucion2456[PROGRESO])</f>
         <v>0</v>
       </c>
     </row>
@@ -2893,7 +3296,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="2">
-        <f>COUNTIF(Distribucion24[ESTADO],"HACER")</f>
+        <f>COUNTIF(Distribucion2456[ESTADO],"HACER")</f>
         <v>0</v>
       </c>
       <c r="G11" s="16" t="s">
@@ -2911,7 +3314,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="2">
-        <f>COUNTIF(Distribucion24[ESTADO],"HACIENDO")</f>
+        <f>COUNTIF(Distribucion2456[ESTADO],"HACIENDO")</f>
         <v>7</v>
       </c>
       <c r="G12" s="20">
@@ -2929,7 +3332,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <f>COUNTIF(Distribucion24[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Distribucion2456[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="G13" s="20">
@@ -2947,7 +3350,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2">
-        <f>COUNTIF(Distribucion24[ESTADO],"HECHO")</f>
+        <f>COUNTIF(Distribucion2456[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
       <c r="G14" s="20">
@@ -2965,7 +3368,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="2">
-        <f>COUNTIF(Distribucion24[ESTADO],"POSPUESTO")</f>
+        <f>COUNTIF(Distribucion2456[ESTADO],"POSPUESTO")</f>
         <v>0</v>
       </c>
       <c r="G15" s="20">
@@ -2984,28 +3387,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="expression" dxfId="39" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="106" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3030,7 +3433,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,10 +3478,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3094,10 +3497,10 @@
         <v>43</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3113,10 +3516,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F4" s="5" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3132,10 +3535,10 @@
         <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3151,10 +3554,10 @@
         <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F6" s="5" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="6"/>
@@ -3171,10 +3574,10 @@
         <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F7" s="26" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3190,10 +3593,10 @@
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F8" s="26" t="str">
-        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion245[[#This Row],[ESTADO]]="HECHO",Distribucion245[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3202,7 +3605,7 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="F9" s="6">
-        <f>SUBTOTAL(109,Distribucion2[PROGRESO])</f>
+        <f>SUBTOTAL(109,Distribucion245[PROGRESO])</f>
         <v>0</v>
       </c>
     </row>
@@ -3211,8 +3614,8 @@
         <v>11</v>
       </c>
       <c r="D11" s="2">
-        <f>COUNTIF(Distribucion2[ESTADO],"HACER")</f>
-        <v>7</v>
+        <f>COUNTIF(Distribucion245[ESTADO],"HACER")</f>
+        <v>0</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>18</v>
@@ -3229,8 +3632,8 @@
         <v>12</v>
       </c>
       <c r="D12" s="2">
-        <f>COUNTIF(Distribucion2[ESTADO],"HACIENDO")</f>
-        <v>0</v>
+        <f>COUNTIF(Distribucion245[ESTADO],"HACIENDO")</f>
+        <v>7</v>
       </c>
       <c r="G12" s="20">
         <v>1</v>
@@ -3247,7 +3650,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <f>COUNTIF(Distribucion2[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Distribucion245[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="G13" s="20">
@@ -3265,7 +3668,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2">
-        <f>COUNTIF(Distribucion2[ESTADO],"HECHO")</f>
+        <f>COUNTIF(Distribucion245[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
       <c r="G14" s="20">
@@ -3283,7 +3686,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="2">
-        <f>COUNTIF(Distribucion2[ESTADO],"POSPUESTO")</f>
+        <f>COUNTIF(Distribucion245[ESTADO],"POSPUESTO")</f>
         <v>0</v>
       </c>
       <c r="G15" s="20">
@@ -3301,44 +3704,30 @@
       <c r="H19" s="17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="79" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="E2:E8">
+    <cfRule type="expression" dxfId="93" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="75" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="expression" dxfId="72" priority="1" stopIfTrue="1">
-      <formula>($E3="VERIFICAR")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="2" stopIfTrue="1">
-      <formula>($E3="HECHO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="3" stopIfTrue="1">
-      <formula>($E3="HACIENDO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="4" stopIfTrue="1">
-      <formula>($E3="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -3362,6 +3751,656 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="9" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="5" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="26" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="26" t="str">
+        <f>IF(Distribucion24[[#This Row],[ESTADO]]="HECHO",Distribucion24[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="6">
+        <f>SUBTOTAL(109,Distribucion24[PROGRESO])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <f>COUNTIF(Distribucion24[ESTADO],"HACER")</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <f>COUNTIF(Distribucion24[ESTADO],"HACIENDO")</f>
+        <v>7</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
+        <f>COUNTIF(Distribucion24[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="20">
+        <v>2</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <f>COUNTIF(Distribucion24[ESTADO],"HECHO")</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="20">
+        <v>3</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2">
+        <f>COUNTIF(Distribucion24[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="20">
+        <v>4</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E8">
+    <cfRule type="expression" dxfId="75" priority="8" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="9" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="10" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="11" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="71" priority="5" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="6" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="7" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA, JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="9" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="5" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="26" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="26" t="str">
+        <f>IF(Distribucion2[[#This Row],[ESTADO]]="HECHO",Distribucion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="6">
+        <f>SUBTOTAL(109,Distribucion2[PROGRESO])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <f>COUNTIF(Distribucion2[ESTADO],"HACER")</f>
+        <v>7</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <f>COUNTIF(Distribucion2[ESTADO],"HACIENDO")</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
+        <f>COUNTIF(Distribucion2[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="20">
+        <v>2</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <f>COUNTIF(Distribucion2[ESTADO],"HECHO")</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="20">
+        <v>3</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2">
+        <f>COUNTIF(Distribucion2[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="20">
+        <v>4</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="expression" dxfId="57" priority="8" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="10" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="11" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="53" priority="5" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="6" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="7" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E8">
+    <cfRule type="expression" dxfId="50" priority="1" stopIfTrue="1">
+      <formula>($E3="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="2" stopIfTrue="1">
+      <formula>($E3="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="3" stopIfTrue="1">
+      <formula>($E3="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="4" stopIfTrue="1">
+      <formula>($E3="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA, JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3620,28 +4659,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E7 E2">
-    <cfRule type="expression" dxfId="57" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="53" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>